<commit_message>
Relatório de aletas - TCM
</commit_message>
<xml_diff>
--- a/Lab. TCM I/Relatório_3/Dados_experimento.xlsx
+++ b/Lab. TCM I/Relatório_3/Dados_experimento.xlsx
@@ -5,22 +5,33 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNESP\7-semestre-EngMec\Lab. TCM I\Relatório_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNESP\EngMec-UNESP\Lab. TCM I\Relatório_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E06F697-0AC5-4447-9146-AFC5EFA68A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B934C5-4872-418E-90ED-33B4A0D86414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-156" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26580" yWindow="1524" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Barra1</t>
   </si>
@@ -65,13 +76,16 @@
   </si>
   <si>
     <t>T10</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +95,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,12 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +491,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D2">
+        <v>68.083633333333339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D3">
+        <v>59.944166666666668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D4">
+        <v>52.760000000000012</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0.21</v>
+      </c>
+      <c r="D5">
+        <v>45.257399999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D6">
+        <v>39.859566666666673</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D7">
+        <v>35.098599999999998</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="D8">
+        <v>32.613266666666682</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="D9">
+        <v>32.613266666666682</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="D10">
+        <v>32.613266666666682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="D11">
+        <v>32.613266666666682</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9CCD55-1B22-4CB7-96DD-4FED8630A06A}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -500,7 +695,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>68.083633333333339</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D2">
         <v>76.005633333333336</v>
@@ -520,7 +715,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59.944166666666668</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D3">
         <v>66.204099999999997</v>
@@ -540,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>52.760000000000012</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D4">
         <v>57.963666666666668</v>
@@ -560,7 +755,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>45.257399999999997</v>
+        <v>0.21</v>
       </c>
       <c r="D5">
         <v>48.729100000000003</v>
@@ -580,7 +775,7 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>39.859566666666673</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D6">
         <v>41.242033333333332</v>
@@ -600,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>35.098599999999998</v>
+        <v>0.41</v>
       </c>
       <c r="D7">
         <v>34.081166666666668</v>
@@ -620,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>32.613266666666682</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="D8">
         <v>29.312433333333338</v>
@@ -640,12 +835,12 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1.5</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="D9">
         <v>27.30863333333334</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>32.931700000000014</v>
       </c>
       <c r="F9">
@@ -660,7 +855,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1.5</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="D10">
         <v>25.36619</v>
@@ -680,7 +875,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1.5</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="D11">
         <v>24.334</v>
@@ -692,8 +887,11 @@
         <v>23.37093333333333</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="3"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>